<commit_message>
Adicionado o projeto CRUD-JAVA da BinaTur.
</commit_message>
<xml_diff>
--- a/uml_BINATUR/dicDadosUml/Dicionário_de_Dados_UML.xlsx
+++ b/uml_BINATUR/dicDadosUml/Dicionário_de_Dados_UML.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dante\OneDrive\Área de Trabalho\RECODE\HardSkills\2.HTML_CSS\BINA-TUR_Site\uml_BINATUR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d338adc7bd1f427a/Área de Trabalho/RECODE/HardSkills/2.HTML_CSS/BINA-TUR_Site/uml_BINATUR/dicDadosUml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BFD4DD-E344-4F97-8BF0-4D409D3589A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{C7BFD4DD-E344-4F97-8BF0-4D409D3589A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8360DB8F-9F9B-43C6-892D-4827B5833FE6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{3753AB37-A9DF-4370-90F2-7F33F0B6C4D3}"/>
   </bookViews>
@@ -1860,7 +1860,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2006,359 +2006,356 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2697,10 +2694,10 @@
   <dimension ref="A1:M62"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F67" sqref="F67"/>
+      <selection pane="bottomRight" activeCell="J62" sqref="A6:J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2718,38 +2715,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="155" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="50"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="156"/>
+      <c r="F1" s="156"/>
+      <c r="G1" s="156"/>
+      <c r="H1" s="156"/>
+      <c r="I1" s="156"/>
+      <c r="J1" s="157"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="60" t="s">
+      <c r="C2" s="135"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="149" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="82"/>
-      <c r="J2" s="61"/>
+      <c r="I2" s="150"/>
+      <c r="J2" s="151"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -2758,80 +2755,80 @@
       <c r="A3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="139" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="63"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="141"/>
+      <c r="F3" s="142"/>
+      <c r="G3" s="143"/>
+      <c r="H3" s="152"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="154"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="137" t="s">
+      <c r="B4" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="63"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="146"/>
+      <c r="E4" s="146"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="148"/>
+      <c r="H4" s="152"/>
+      <c r="I4" s="153"/>
+      <c r="J4" s="154"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="95" t="s">
+      <c r="A5" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="77" t="s">
+      <c r="C5" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="77" t="s">
+      <c r="D5" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="78" t="s">
+      <c r="E5" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="136" t="s">
+      <c r="F5" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="79" t="s">
+      <c r="G5" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="79" t="s">
+      <c r="H5" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="96" t="s">
+      <c r="I5" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="97" t="s">
+      <c r="J5" s="64" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="131" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="138" t="s">
+      <c r="B6" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="139" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="87" t="s">
+      <c r="C6" s="93" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="56" t="s">
         <v>43</v>
       </c>
       <c r="E6" s="43" t="s">
@@ -2840,7 +2837,7 @@
       <c r="F6" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="93" t="s">
+      <c r="G6" s="60" t="s">
         <v>36</v>
       </c>
       <c r="H6" s="42" t="s">
@@ -2849,16 +2846,16 @@
       <c r="I6" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="88" t="s">
+      <c r="J6" s="57" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="84"/>
+      <c r="A7" s="132"/>
       <c r="B7" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="91" t="s">
+      <c r="C7" s="58" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="12" t="s">
@@ -2879,16 +2876,16 @@
       <c r="I7" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="88" t="s">
+      <c r="J7" s="57" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="85"/>
+      <c r="A8" s="133"/>
       <c r="B8" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="92" t="s">
+      <c r="C8" s="59" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="14" t="s">
@@ -2914,37 +2911,37 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="59"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
+      <c r="A9" s="129"/>
+      <c r="B9" s="129"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="129"/>
+      <c r="E9" s="129"/>
+      <c r="F9" s="130"/>
+      <c r="G9" s="130"/>
+      <c r="H9" s="130"/>
+      <c r="I9" s="130"/>
+      <c r="J9" s="130"/>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="99" t="s">
+      <c r="A10" s="126" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="100" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="101" t="s">
+      <c r="C10" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="102" t="s">
+      <c r="E10" s="68" t="s">
         <v>35</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="103" t="s">
+      <c r="G10" s="69" t="s">
         <v>36</v>
       </c>
       <c r="H10" s="17" t="s">
@@ -2958,29 +2955,29 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="104"/>
-      <c r="B11" s="105" t="s">
+      <c r="A11" s="127"/>
+      <c r="B11" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="106" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="107" t="s">
+      <c r="C11" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="108" t="s">
+      <c r="E11" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="105" t="s">
+      <c r="F11" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="107" t="s">
+      <c r="G11" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="109" t="s">
+      <c r="H11" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="I11" s="109" t="s">
+      <c r="I11" s="74" t="s">
         <v>70</v>
       </c>
       <c r="J11" s="31" t="s">
@@ -2988,29 +2985,29 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="104"/>
-      <c r="B12" s="105" t="s">
+      <c r="A12" s="127"/>
+      <c r="B12" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="106" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="107" t="s">
+      <c r="C12" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="108" t="s">
+      <c r="E12" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="105" t="s">
+      <c r="F12" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="107" t="s">
+      <c r="G12" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="109" t="s">
+      <c r="H12" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="I12" s="109" t="s">
+      <c r="I12" s="74" t="s">
         <v>72</v>
       </c>
       <c r="J12" s="31" t="s">
@@ -3018,11 +3015,11 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="104"/>
+      <c r="A13" s="127"/>
       <c r="B13" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="110" t="s">
+      <c r="C13" s="75" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -3048,11 +3045,11 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="104"/>
+      <c r="A14" s="127"/>
       <c r="B14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="110" t="s">
+      <c r="C14" s="75" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="6" t="s">
@@ -3078,11 +3075,11 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="104"/>
+      <c r="A15" s="127"/>
       <c r="B15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="110" t="s">
+      <c r="C15" s="75" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="6" t="s">
@@ -3108,11 +3105,11 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="111"/>
+      <c r="A16" s="128"/>
       <c r="B16" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="112" t="s">
+      <c r="C16" s="76" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="9" t="s">
@@ -3121,10 +3118,10 @@
       <c r="E16" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="113" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="114" t="s">
+      <c r="F16" s="77" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="78" t="s">
         <v>69</v>
       </c>
       <c r="H16" s="47" t="s">
@@ -3138,37 +3135,37 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="59"/>
-      <c r="B17" s="76"/>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="76"/>
-      <c r="I17" s="76"/>
-      <c r="J17" s="76"/>
+      <c r="A17" s="129"/>
+      <c r="B17" s="130"/>
+      <c r="C17" s="130"/>
+      <c r="D17" s="130"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="130"/>
+      <c r="G17" s="130"/>
+      <c r="H17" s="130"/>
+      <c r="I17" s="130"/>
+      <c r="J17" s="130"/>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="115" t="s">
+      <c r="A18" s="123" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="128" t="s">
+      <c r="C18" s="83" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="74" t="s">
+      <c r="E18" s="50" t="s">
         <v>89</v>
       </c>
       <c r="F18" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="129" t="s">
+      <c r="G18" s="84" t="s">
         <v>36</v>
       </c>
       <c r="H18" s="20" t="s">
@@ -3182,11 +3179,11 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="116"/>
+      <c r="A19" s="124"/>
       <c r="B19" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="117" t="s">
+      <c r="C19" s="79" t="s">
         <v>32</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -3212,11 +3209,11 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="116"/>
+      <c r="A20" s="124"/>
       <c r="B20" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="117" t="s">
+      <c r="C20" s="79" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -3242,20 +3239,20 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="118"/>
+      <c r="A21" s="125"/>
       <c r="B21" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="119" t="s">
+      <c r="C21" s="80" t="s">
         <v>32</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="75" t="s">
+      <c r="E21" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="130" t="s">
+      <c r="F21" s="85" t="s">
         <v>14</v>
       </c>
       <c r="G21" s="22" t="s">
@@ -3267,42 +3264,42 @@
       <c r="I21" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="J21" s="98" t="s">
+      <c r="J21" s="65" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="120"/>
-      <c r="B22" s="120"/>
-      <c r="C22" s="120"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="120"/>
-      <c r="G22" s="120"/>
-      <c r="H22" s="120"/>
-      <c r="I22" s="120"/>
-      <c r="J22" s="120"/>
+      <c r="A22" s="122"/>
+      <c r="B22" s="122"/>
+      <c r="C22" s="122"/>
+      <c r="D22" s="122"/>
+      <c r="E22" s="122"/>
+      <c r="F22" s="122"/>
+      <c r="G22" s="122"/>
+      <c r="H22" s="122"/>
+      <c r="I22" s="122"/>
+      <c r="J22" s="122"/>
     </row>
     <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="121" t="s">
+      <c r="A23" s="118" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="C23" s="133" t="s">
+      <c r="C23" s="88" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="E23" s="73" t="s">
+      <c r="E23" s="49" t="s">
         <v>35</v>
       </c>
       <c r="F23" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="G23" s="134" t="s">
+      <c r="G23" s="89" t="s">
         <v>36</v>
       </c>
       <c r="H23" s="18" t="s">
@@ -3316,11 +3313,11 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="122"/>
+      <c r="A24" s="119"/>
       <c r="B24" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="123" t="s">
+      <c r="C24" s="81" t="s">
         <v>32</v>
       </c>
       <c r="D24" s="7" t="s">
@@ -3346,11 +3343,11 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="122"/>
+      <c r="A25" s="119"/>
       <c r="B25" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C25" s="123" t="s">
+      <c r="C25" s="81" t="s">
         <v>32</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -3376,17 +3373,17 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="124"/>
+      <c r="A26" s="120"/>
       <c r="B26" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="131" t="s">
+      <c r="C26" s="86" t="s">
         <v>69</v>
       </c>
       <c r="D26" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="132" t="s">
+      <c r="E26" s="87" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="32" t="s">
@@ -3406,37 +3403,37 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="120"/>
-      <c r="B27" s="120"/>
-      <c r="C27" s="120"/>
-      <c r="D27" s="120"/>
-      <c r="E27" s="120"/>
-      <c r="F27" s="120"/>
-      <c r="G27" s="120"/>
-      <c r="H27" s="120"/>
-      <c r="I27" s="120"/>
-      <c r="J27" s="120"/>
+      <c r="A27" s="122"/>
+      <c r="B27" s="122"/>
+      <c r="C27" s="122"/>
+      <c r="D27" s="122"/>
+      <c r="E27" s="122"/>
+      <c r="F27" s="122"/>
+      <c r="G27" s="122"/>
+      <c r="H27" s="122"/>
+      <c r="I27" s="122"/>
+      <c r="J27" s="122"/>
     </row>
     <row r="28" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="115" t="s">
+      <c r="A28" s="123" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="C28" s="128" t="s">
+      <c r="C28" s="83" t="s">
         <v>32</v>
       </c>
       <c r="D28" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="E28" s="74" t="s">
+      <c r="E28" s="50" t="s">
         <v>38</v>
       </c>
       <c r="F28" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G28" s="129" t="s">
+      <c r="G28" s="84" t="s">
         <v>36</v>
       </c>
       <c r="H28" s="20" t="s">
@@ -3450,11 +3447,11 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="116"/>
+      <c r="A29" s="124"/>
       <c r="B29" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="C29" s="117" t="s">
+      <c r="C29" s="79" t="s">
         <v>32</v>
       </c>
       <c r="D29" s="3" t="s">
@@ -3480,11 +3477,11 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="116"/>
+      <c r="A30" s="124"/>
       <c r="B30" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C30" s="117" t="s">
+      <c r="C30" s="79" t="s">
         <v>32</v>
       </c>
       <c r="D30" s="3" t="s">
@@ -3510,11 +3507,11 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="116"/>
+      <c r="A31" s="124"/>
       <c r="B31" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="C31" s="117" t="s">
+      <c r="C31" s="79" t="s">
         <v>32</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -3540,11 +3537,11 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="116"/>
+      <c r="A32" s="124"/>
       <c r="B32" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="C32" s="117" t="s">
+      <c r="C32" s="79" t="s">
         <v>32</v>
       </c>
       <c r="D32" s="3" t="s">
@@ -3570,20 +3567,20 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="118"/>
+      <c r="A33" s="125"/>
       <c r="B33" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C33" s="119" t="s">
+      <c r="C33" s="80" t="s">
         <v>32</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E33" s="75" t="s">
+      <c r="E33" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="F33" s="130" t="s">
+      <c r="F33" s="85" t="s">
         <v>14</v>
       </c>
       <c r="G33" s="22" t="s">
@@ -3595,42 +3592,42 @@
       <c r="I33" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="J33" s="98" t="s">
+      <c r="J33" s="65" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="126"/>
-      <c r="B34" s="126"/>
-      <c r="C34" s="126"/>
-      <c r="D34" s="126"/>
-      <c r="E34" s="126"/>
-      <c r="F34" s="127"/>
-      <c r="G34" s="127"/>
-      <c r="H34" s="127"/>
-      <c r="I34" s="127"/>
-      <c r="J34" s="127"/>
-    </row>
-    <row r="35" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A35" s="121" t="s">
+      <c r="A34" s="121"/>
+      <c r="B34" s="121"/>
+      <c r="C34" s="121"/>
+      <c r="D34" s="121"/>
+      <c r="E34" s="121"/>
+      <c r="F34" s="122"/>
+      <c r="G34" s="122"/>
+      <c r="H34" s="122"/>
+      <c r="I34" s="122"/>
+      <c r="J34" s="122"/>
+    </row>
+    <row r="35" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A35" s="118" t="s">
         <v>8</v>
       </c>
       <c r="B35" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="C35" s="133" t="s">
+      <c r="C35" s="88" t="s">
         <v>32</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="E35" s="73" t="s">
+      <c r="E35" s="49" t="s">
         <v>38</v>
       </c>
       <c r="F35" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="G35" s="134" t="s">
+      <c r="G35" s="89" t="s">
         <v>36</v>
       </c>
       <c r="H35" s="18" t="s">
@@ -3643,12 +3640,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A36" s="122"/>
+    <row r="36" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A36" s="119"/>
       <c r="B36" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="C36" s="123" t="s">
+      <c r="C36" s="81" t="s">
         <v>32</v>
       </c>
       <c r="D36" s="7" t="s">
@@ -3674,11 +3671,11 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="122"/>
+      <c r="A37" s="119"/>
       <c r="B37" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="C37" s="123" t="s">
+      <c r="C37" s="81" t="s">
         <v>32</v>
       </c>
       <c r="D37" s="7" t="s">
@@ -3702,11 +3699,11 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="122"/>
+      <c r="A38" s="119"/>
       <c r="B38" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="C38" s="123" t="s">
+      <c r="C38" s="81" t="s">
         <v>32</v>
       </c>
       <c r="D38" s="7" t="s">
@@ -3718,13 +3715,13 @@
       <c r="F38" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="G38" s="135" t="s">
+      <c r="G38" s="90" t="s">
         <v>69</v>
       </c>
-      <c r="H38" s="135" t="s">
-        <v>14</v>
-      </c>
-      <c r="I38" s="135" t="s">
+      <c r="H38" s="90" t="s">
+        <v>14</v>
+      </c>
+      <c r="I38" s="90" t="s">
         <v>14</v>
       </c>
       <c r="J38" s="38" t="s">
@@ -3732,11 +3729,11 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="122"/>
+      <c r="A39" s="119"/>
       <c r="B39" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="C39" s="123" t="s">
+      <c r="C39" s="81" t="s">
         <v>32</v>
       </c>
       <c r="D39" s="7" t="s">
@@ -3762,11 +3759,11 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="122"/>
+      <c r="A40" s="119"/>
       <c r="B40" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="C40" s="123" t="s">
+      <c r="C40" s="81" t="s">
         <v>32</v>
       </c>
       <c r="D40" s="7" t="s">
@@ -3792,11 +3789,11 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="122"/>
+      <c r="A41" s="119"/>
       <c r="B41" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="C41" s="123" t="s">
+      <c r="C41" s="81" t="s">
         <v>32</v>
       </c>
       <c r="D41" s="7" t="s">
@@ -3822,11 +3819,11 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="122"/>
+      <c r="A42" s="119"/>
       <c r="B42" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="C42" s="123" t="s">
+      <c r="C42" s="81" t="s">
         <v>32</v>
       </c>
       <c r="D42" s="7" t="s">
@@ -3852,11 +3849,11 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="124"/>
+      <c r="A43" s="120"/>
       <c r="B43" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="C43" s="125" t="s">
+      <c r="C43" s="82" t="s">
         <v>32</v>
       </c>
       <c r="D43" s="10" t="s">
@@ -3882,37 +3879,37 @@
       </c>
     </row>
     <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="126"/>
-      <c r="B44" s="126"/>
-      <c r="C44" s="126"/>
-      <c r="D44" s="126"/>
-      <c r="E44" s="126"/>
-      <c r="F44" s="127"/>
-      <c r="G44" s="127"/>
-      <c r="H44" s="127"/>
-      <c r="I44" s="127"/>
-      <c r="J44" s="127"/>
+      <c r="A44" s="121"/>
+      <c r="B44" s="121"/>
+      <c r="C44" s="121"/>
+      <c r="D44" s="121"/>
+      <c r="E44" s="121"/>
+      <c r="F44" s="122"/>
+      <c r="G44" s="122"/>
+      <c r="H44" s="122"/>
+      <c r="I44" s="122"/>
+      <c r="J44" s="122"/>
     </row>
     <row r="45" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A45" s="115" t="s">
+      <c r="A45" s="123" t="s">
         <v>10</v>
       </c>
       <c r="B45" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="C45" s="128" t="s">
+      <c r="C45" s="83" t="s">
         <v>32</v>
       </c>
       <c r="D45" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="E45" s="74" t="s">
+      <c r="E45" s="50" t="s">
         <v>38</v>
       </c>
       <c r="F45" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="G45" s="129" t="s">
+      <c r="G45" s="84" t="s">
         <v>36</v>
       </c>
       <c r="H45" s="20" t="s">
@@ -3926,11 +3923,11 @@
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="116"/>
+      <c r="A46" s="124"/>
       <c r="B46" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="C46" s="117" t="s">
+      <c r="C46" s="79" t="s">
         <v>32</v>
       </c>
       <c r="D46" s="3" t="s">
@@ -3956,11 +3953,11 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="116"/>
+      <c r="A47" s="124"/>
       <c r="B47" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="C47" s="117" t="s">
+      <c r="C47" s="79" t="s">
         <v>32</v>
       </c>
       <c r="D47" s="3" t="s">
@@ -3986,11 +3983,11 @@
       </c>
     </row>
     <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="116"/>
+      <c r="A48" s="124"/>
       <c r="B48" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="C48" s="117" t="s">
+      <c r="C48" s="79" t="s">
         <v>32</v>
       </c>
       <c r="D48" s="3" t="s">
@@ -3999,28 +3996,28 @@
       <c r="E48" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="F48" s="140" t="s">
-        <v>14</v>
-      </c>
-      <c r="G48" s="141" t="s">
+      <c r="F48" s="94" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="H48" s="141" t="s">
-        <v>14</v>
-      </c>
-      <c r="I48" s="141" t="s">
-        <v>14</v>
-      </c>
-      <c r="J48" s="142" t="s">
+      <c r="H48" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="I48" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="J48" s="96" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="116"/>
+      <c r="A49" s="124"/>
       <c r="B49" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="C49" s="117" t="s">
+      <c r="C49" s="79" t="s">
         <v>32</v>
       </c>
       <c r="D49" s="3" t="s">
@@ -4029,84 +4026,84 @@
       <c r="E49" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="F49" s="140" t="s">
-        <v>14</v>
-      </c>
-      <c r="G49" s="141" t="s">
+      <c r="F49" s="94" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="H49" s="141" t="s">
-        <v>14</v>
-      </c>
-      <c r="I49" s="141" t="s">
-        <v>14</v>
-      </c>
-      <c r="J49" s="142" t="s">
+      <c r="H49" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="I49" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="J49" s="96" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="118"/>
+      <c r="A50" s="125"/>
       <c r="B50" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="C50" s="119" t="s">
+      <c r="C50" s="80" t="s">
         <v>32</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E50" s="75" t="s">
+      <c r="E50" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="F50" s="143" t="s">
-        <v>14</v>
-      </c>
-      <c r="G50" s="144" t="s">
+      <c r="F50" s="97" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" s="98" t="s">
         <v>69</v>
       </c>
-      <c r="H50" s="144" t="s">
-        <v>14</v>
-      </c>
-      <c r="I50" s="144" t="s">
-        <v>14</v>
-      </c>
-      <c r="J50" s="145" t="s">
+      <c r="H50" s="98" t="s">
+        <v>14</v>
+      </c>
+      <c r="I50" s="98" t="s">
+        <v>14</v>
+      </c>
+      <c r="J50" s="99" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="126"/>
-      <c r="B51" s="126"/>
-      <c r="C51" s="126"/>
-      <c r="D51" s="126"/>
-      <c r="E51" s="126"/>
-      <c r="F51" s="127"/>
-      <c r="G51" s="127"/>
-      <c r="H51" s="127"/>
-      <c r="I51" s="127"/>
-      <c r="J51" s="127"/>
+      <c r="A51" s="121"/>
+      <c r="B51" s="121"/>
+      <c r="C51" s="121"/>
+      <c r="D51" s="121"/>
+      <c r="E51" s="121"/>
+      <c r="F51" s="122"/>
+      <c r="G51" s="122"/>
+      <c r="H51" s="122"/>
+      <c r="I51" s="122"/>
+      <c r="J51" s="122"/>
     </row>
     <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A52" s="121" t="s">
+      <c r="A52" s="118" t="s">
         <v>27</v>
       </c>
       <c r="B52" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="C52" s="133" t="s">
+      <c r="C52" s="88" t="s">
         <v>32</v>
       </c>
       <c r="D52" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="E52" s="73" t="s">
+      <c r="E52" s="49" t="s">
         <v>90</v>
       </c>
       <c r="F52" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="G52" s="134" t="s">
+      <c r="G52" s="89" t="s">
         <v>36</v>
       </c>
       <c r="H52" s="18" t="s">
@@ -4120,11 +4117,11 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="122"/>
+      <c r="A53" s="119"/>
       <c r="B53" s="30" t="s">
         <v>173</v>
       </c>
-      <c r="C53" s="123" t="s">
+      <c r="C53" s="81" t="s">
         <v>32</v>
       </c>
       <c r="D53" s="7" t="s">
@@ -4150,11 +4147,11 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="122"/>
+      <c r="A54" s="119"/>
       <c r="B54" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="C54" s="123" t="s">
+      <c r="C54" s="81" t="s">
         <v>32</v>
       </c>
       <c r="D54" s="7" t="s">
@@ -4180,11 +4177,11 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="124"/>
+      <c r="A55" s="120"/>
       <c r="B55" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="C55" s="125" t="s">
+      <c r="C55" s="82" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="10" t="s">
@@ -4210,37 +4207,37 @@
       </c>
     </row>
     <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="126"/>
-      <c r="B56" s="126"/>
-      <c r="C56" s="126"/>
-      <c r="D56" s="126"/>
-      <c r="E56" s="126"/>
-      <c r="F56" s="127"/>
-      <c r="G56" s="127"/>
-      <c r="H56" s="127"/>
-      <c r="I56" s="127"/>
-      <c r="J56" s="127"/>
+      <c r="A56" s="121"/>
+      <c r="B56" s="121"/>
+      <c r="C56" s="121"/>
+      <c r="D56" s="121"/>
+      <c r="E56" s="121"/>
+      <c r="F56" s="122"/>
+      <c r="G56" s="122"/>
+      <c r="H56" s="122"/>
+      <c r="I56" s="122"/>
+      <c r="J56" s="122"/>
     </row>
     <row r="57" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A57" s="115" t="s">
+      <c r="A57" s="123" t="s">
         <v>28</v>
       </c>
       <c r="B57" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="C57" s="128" t="s">
+      <c r="C57" s="83" t="s">
         <v>32</v>
       </c>
       <c r="D57" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E57" s="74" t="s">
+      <c r="E57" s="50" t="s">
         <v>90</v>
       </c>
       <c r="F57" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="G57" s="129" t="s">
+      <c r="G57" s="84" t="s">
         <v>36</v>
       </c>
       <c r="H57" s="20"/>
@@ -4252,11 +4249,11 @@
       </c>
     </row>
     <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="116"/>
+      <c r="A58" s="124"/>
       <c r="B58" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="C58" s="117" t="s">
+      <c r="C58" s="79" t="s">
         <v>32</v>
       </c>
       <c r="D58" s="3" t="s">
@@ -4265,28 +4262,28 @@
       <c r="E58" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="F58" s="140" t="s">
-        <v>14</v>
-      </c>
-      <c r="G58" s="141" t="s">
+      <c r="F58" s="94" t="s">
+        <v>14</v>
+      </c>
+      <c r="G58" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="H58" s="141" t="s">
-        <v>14</v>
-      </c>
-      <c r="I58" s="141" t="s">
-        <v>14</v>
-      </c>
-      <c r="J58" s="142" t="s">
+      <c r="H58" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="I58" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="J58" s="96" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="116"/>
+      <c r="A59" s="124"/>
       <c r="B59" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="C59" s="117" t="s">
+      <c r="C59" s="79" t="s">
         <v>32</v>
       </c>
       <c r="D59" s="3" t="s">
@@ -4295,28 +4292,28 @@
       <c r="E59" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="F59" s="140" t="s">
-        <v>14</v>
-      </c>
-      <c r="G59" s="141" t="s">
+      <c r="F59" s="94" t="s">
+        <v>14</v>
+      </c>
+      <c r="G59" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="H59" s="141" t="s">
-        <v>14</v>
-      </c>
-      <c r="I59" s="141" t="s">
-        <v>14</v>
-      </c>
-      <c r="J59" s="142" t="s">
+      <c r="H59" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="I59" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="J59" s="96" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="116"/>
+      <c r="A60" s="124"/>
       <c r="B60" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="C60" s="117" t="s">
+      <c r="C60" s="79" t="s">
         <v>32</v>
       </c>
       <c r="D60" s="3" t="s">
@@ -4325,28 +4322,28 @@
       <c r="E60" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="F60" s="140" t="s">
-        <v>14</v>
-      </c>
-      <c r="G60" s="141" t="s">
+      <c r="F60" s="94" t="s">
+        <v>14</v>
+      </c>
+      <c r="G60" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="H60" s="141" t="s">
-        <v>14</v>
-      </c>
-      <c r="I60" s="141" t="s">
-        <v>14</v>
-      </c>
-      <c r="J60" s="142" t="s">
+      <c r="H60" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="I60" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="J60" s="96" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="116"/>
+      <c r="A61" s="124"/>
       <c r="B61" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="C61" s="117" t="s">
+      <c r="C61" s="79" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="3" t="s">
@@ -4355,54 +4352,65 @@
       <c r="E61" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="F61" s="140" t="s">
-        <v>14</v>
-      </c>
-      <c r="G61" s="141" t="s">
+      <c r="F61" s="94" t="s">
+        <v>14</v>
+      </c>
+      <c r="G61" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="H61" s="141" t="s">
-        <v>14</v>
-      </c>
-      <c r="I61" s="141" t="s">
-        <v>14</v>
-      </c>
-      <c r="J61" s="142" t="s">
+      <c r="H61" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="I61" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="J61" s="96" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="118"/>
+      <c r="A62" s="125"/>
       <c r="B62" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="C62" s="119" t="s">
+      <c r="C62" s="80" t="s">
         <v>32</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="E62" s="75" t="s">
+      <c r="E62" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="F62" s="143" t="s">
-        <v>14</v>
-      </c>
-      <c r="G62" s="144" t="s">
+      <c r="F62" s="97" t="s">
+        <v>14</v>
+      </c>
+      <c r="G62" s="98" t="s">
         <v>69</v>
       </c>
-      <c r="H62" s="146" t="s">
-        <v>14</v>
-      </c>
-      <c r="I62" s="144" t="s">
-        <v>14</v>
-      </c>
-      <c r="J62" s="145" t="s">
+      <c r="H62" s="100" t="s">
+        <v>14</v>
+      </c>
+      <c r="I62" s="98" t="s">
+        <v>14</v>
+      </c>
+      <c r="J62" s="99" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="H2:J4"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A35:A43"/>
     <mergeCell ref="A52:A55"/>
     <mergeCell ref="A56:J56"/>
     <mergeCell ref="A57:A62"/>
@@ -4411,20 +4419,9 @@
     <mergeCell ref="A27:J27"/>
     <mergeCell ref="A28:A33"/>
     <mergeCell ref="A34:J34"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="A17:J17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A35:A43"/>
     <mergeCell ref="A44:J44"/>
     <mergeCell ref="A45:A50"/>
     <mergeCell ref="A51:J51"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="H2:J4"/>
-    <mergeCell ref="B1:J1"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="71" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -4439,10 +4436,10 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="A6:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4455,26 +4452,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="156" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="157"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="158" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="148" t="s">
+      <c r="C2" s="159"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="161" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="1"/>
@@ -4486,195 +4483,195 @@
       <c r="A3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="141" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="149"/>
+      <c r="C3" s="141"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="162"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="164" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="150"/>
+      <c r="C4" s="164"/>
+      <c r="D4" s="165"/>
+      <c r="E4" s="163"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="163" t="s">
+      <c r="A5" s="114" t="s">
         <v>196</v>
       </c>
-      <c r="B5" s="164" t="s">
+      <c r="B5" s="115" t="s">
         <v>198</v>
       </c>
-      <c r="C5" s="165" t="s">
+      <c r="C5" s="116" t="s">
         <v>199</v>
       </c>
-      <c r="D5" s="164" t="s">
+      <c r="D5" s="115" t="s">
         <v>197</v>
       </c>
-      <c r="E5" s="165" t="s">
+      <c r="E5" s="116" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="151" t="s">
+      <c r="A6" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="152" t="s">
+      <c r="B6" s="103" t="s">
         <v>201</v>
       </c>
-      <c r="C6" s="152" t="s">
+      <c r="C6" s="103" t="s">
         <v>227</v>
       </c>
-      <c r="D6" s="152" t="s">
+      <c r="D6" s="103" t="s">
         <v>202</v>
       </c>
-      <c r="E6" s="153" t="s">
+      <c r="E6" s="104" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="154" t="s">
+      <c r="A7" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="155" t="s">
+      <c r="B7" s="106" t="s">
         <v>205</v>
       </c>
-      <c r="C7" s="166" t="s">
+      <c r="C7" s="117" t="s">
         <v>228</v>
       </c>
-      <c r="D7" s="155" t="s">
+      <c r="D7" s="106" t="s">
         <v>225</v>
       </c>
-      <c r="E7" s="156" t="s">
+      <c r="E7" s="107" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="157" t="s">
+      <c r="A8" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="158" t="s">
+      <c r="B8" s="109" t="s">
         <v>207</v>
       </c>
-      <c r="C8" s="158" t="s">
+      <c r="C8" s="109" t="s">
         <v>229</v>
       </c>
-      <c r="D8" s="158" t="s">
+      <c r="D8" s="109" t="s">
         <v>226</v>
       </c>
-      <c r="E8" s="159" t="s">
+      <c r="E8" s="110" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="154" t="s">
+      <c r="A9" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="155" t="s">
+      <c r="B9" s="106" t="s">
         <v>201</v>
       </c>
-      <c r="C9" s="155" t="s">
+      <c r="C9" s="106" t="s">
         <v>230</v>
       </c>
-      <c r="D9" s="155" t="s">
+      <c r="D9" s="106" t="s">
         <v>202</v>
       </c>
-      <c r="E9" s="156" t="s">
+      <c r="E9" s="107" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="157" t="s">
+      <c r="A10" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="158" t="s">
+      <c r="B10" s="109" t="s">
         <v>209</v>
       </c>
-      <c r="C10" s="158" t="s">
+      <c r="C10" s="109" t="s">
         <v>231</v>
       </c>
-      <c r="D10" s="158" t="s">
+      <c r="D10" s="109" t="s">
         <v>210</v>
       </c>
-      <c r="E10" s="159" t="s">
+      <c r="E10" s="110" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="154" t="s">
+      <c r="A11" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="155" t="s">
+      <c r="B11" s="106" t="s">
         <v>216</v>
       </c>
-      <c r="C11" s="155" t="s">
+      <c r="C11" s="106" t="s">
         <v>232</v>
       </c>
-      <c r="D11" s="155" t="s">
+      <c r="D11" s="106" t="s">
         <v>217</v>
       </c>
-      <c r="E11" s="156" t="s">
+      <c r="E11" s="107" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="157" t="s">
+      <c r="A12" s="108" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="158" t="s">
+      <c r="B12" s="109" t="s">
         <v>222</v>
       </c>
-      <c r="C12" s="158" t="s">
+      <c r="C12" s="109" t="s">
         <v>233</v>
       </c>
-      <c r="D12" s="158" t="s">
+      <c r="D12" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="E12" s="159" t="s">
+      <c r="E12" s="110" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="154" t="s">
+      <c r="A13" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="155" t="s">
+      <c r="B13" s="106" t="s">
         <v>213</v>
       </c>
-      <c r="C13" s="155" t="s">
+      <c r="C13" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="D13" s="155" t="s">
+      <c r="D13" s="106" t="s">
         <v>214</v>
       </c>
-      <c r="E13" s="156" t="s">
+      <c r="E13" s="107" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="160" t="s">
+      <c r="A14" s="111" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="161" t="s">
+      <c r="B14" s="112" t="s">
         <v>219</v>
       </c>
-      <c r="C14" s="161" t="s">
+      <c r="C14" s="112" t="s">
         <v>235</v>
       </c>
-      <c r="D14" s="161" t="s">
+      <c r="D14" s="112" t="s">
         <v>220</v>
       </c>
-      <c r="E14" s="162" t="s">
+      <c r="E14" s="113" t="s">
         <v>221</v>
       </c>
     </row>

</xml_diff>